<commit_message>
robot framework folder updated
</commit_message>
<xml_diff>
--- a/Capstone_Project/data/data.xlsx
+++ b/Capstone_Project/data/data.xlsx
@@ -6,9 +6,10 @@
     <sheet state="visible" name="login_data" sheetId="1" r:id="rId5"/>
     <sheet state="visible" name="placeorder_data" sheetId="2" r:id="rId6"/>
     <sheet state="visible" name="pricefilter_data" sheetId="3" r:id="rId7"/>
-    <sheet state="visible" name="productsort_data" sheetId="4" r:id="rId8"/>
-    <sheet state="visible" name="searchproduct_data" sheetId="5" r:id="rId9"/>
+    <sheet state="visible" name="searchproduct_data" sheetId="4" r:id="rId8"/>
+    <sheet state="visible" name="productsort_data" sheetId="5" r:id="rId9"/>
     <sheet state="visible" name="registration_data" sheetId="6" r:id="rId10"/>
+    <sheet state="visible" name="filterorder_data" sheetId="7" r:id="rId11"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="51">
   <si>
     <t>email</t>
   </si>
@@ -36,136 +37,139 @@
     <t>Rani12</t>
   </si>
   <si>
+    <t>Rani16@gmail.com</t>
+  </si>
+  <si>
+    <t>Rani13</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>company</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>zipcode</t>
+  </si>
+  <si>
+    <t>order_notes</t>
+  </si>
+  <si>
+    <t>payment_method</t>
+  </si>
+  <si>
+    <t>Rani</t>
+  </si>
+  <si>
+    <t>Kumari</t>
+  </si>
+  <si>
+    <t>ABC Pvt Ltd</t>
+  </si>
+  <si>
+    <t>rani12@gmail.com</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>Hitech City</t>
+  </si>
+  <si>
+    <t>Hyderabad</t>
+  </si>
+  <si>
+    <t>Telangana</t>
+  </si>
+  <si>
+    <t>"Please deliver between 10 AM - 12 PM"</t>
+  </si>
+  <si>
+    <t>cod</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>XYZ Ltd</t>
+  </si>
+  <si>
+    <t>john@example.com</t>
+  </si>
+  <si>
+    <t>Madhapur</t>
+  </si>
+  <si>
+    <t>"Leave at reception"</t>
+  </si>
+  <si>
+    <t>bacs</t>
+  </si>
+  <si>
+    <t>min_price</t>
+  </si>
+  <si>
+    <t>max_price</t>
+  </si>
+  <si>
+    <t>product_name</t>
+  </si>
+  <si>
+    <t>Selenium Ruby</t>
+  </si>
+  <si>
+    <t>Robot</t>
+  </si>
+  <si>
+    <t>sort_by</t>
+  </si>
+  <si>
+    <t>menu_order</t>
+  </si>
+  <si>
+    <t>popularity</t>
+  </si>
+  <si>
+    <t>rating</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>price-desc</t>
+  </si>
+  <si>
+    <t>Neeraja43@gmail.com</t>
+  </si>
+  <si>
+    <t>Neeraja123@AP</t>
+  </si>
+  <si>
     <t>Rani13@gmail.com</t>
-  </si>
-  <si>
-    <t>Rani13</t>
-  </si>
-  <si>
-    <t>first_name</t>
-  </si>
-  <si>
-    <t>last_name</t>
-  </si>
-  <si>
-    <t>company</t>
-  </si>
-  <si>
-    <t>phone</t>
-  </si>
-  <si>
-    <t>country</t>
-  </si>
-  <si>
-    <t>address</t>
-  </si>
-  <si>
-    <t>city</t>
-  </si>
-  <si>
-    <t>state</t>
-  </si>
-  <si>
-    <t>zipcode</t>
-  </si>
-  <si>
-    <t>order_notes</t>
-  </si>
-  <si>
-    <t>payment_method</t>
-  </si>
-  <si>
-    <t>Rani</t>
-  </si>
-  <si>
-    <t>Kumari</t>
-  </si>
-  <si>
-    <t>ABC Pvt Ltd</t>
-  </si>
-  <si>
-    <t>rani12@gmail.com</t>
-  </si>
-  <si>
-    <t>IN</t>
-  </si>
-  <si>
-    <t>Hitech City</t>
-  </si>
-  <si>
-    <t>Hyderabad</t>
-  </si>
-  <si>
-    <t>Telangana</t>
-  </si>
-  <si>
-    <t>"Please deliver between 10 AM - 12 PM"</t>
-  </si>
-  <si>
-    <t>cod</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Doe</t>
-  </si>
-  <si>
-    <t>XYZ Ltd</t>
-  </si>
-  <si>
-    <t>john@example.com</t>
-  </si>
-  <si>
-    <t>Madhapur</t>
-  </si>
-  <si>
-    <t>"Leave at reception"</t>
-  </si>
-  <si>
-    <t>bacs</t>
-  </si>
-  <si>
-    <t>min_price</t>
-  </si>
-  <si>
-    <t>max_price</t>
-  </si>
-  <si>
-    <t>sort_by</t>
-  </si>
-  <si>
-    <t>menu_order</t>
-  </si>
-  <si>
-    <t>popularity</t>
-  </si>
-  <si>
-    <t>rating</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>price</t>
-  </si>
-  <si>
-    <t>price-desc</t>
-  </si>
-  <si>
-    <t>product_name</t>
-  </si>
-  <si>
-    <t>Selenium Ruby</t>
-  </si>
-  <si>
-    <t>Robot</t>
-  </si>
-  <si>
-    <t>Neeraja12@gmail.com</t>
-  </si>
-  <si>
-    <t>Neeraja123@p</t>
   </si>
 </sst>
 </file>
@@ -249,6 +253,10 @@
 </file>
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -708,26 +716,6 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -745,16 +733,36 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="s">
         <v>47</v>
       </c>
     </row>
@@ -796,4 +804,56 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="15.88"/>
+    <col customWidth="1" min="2" max="2" width="16.0"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>